<commit_message>
agrege EspID a la busqueda de la pagina principal
</commit_message>
<xml_diff>
--- a/Plan De Trabajo Verano.xlsx
+++ b/Plan De Trabajo Verano.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B6E343-D682-43B2-B3A0-A13AFE5B7D4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC5F53F-B930-43B9-AB92-CBC4203C3890}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -1879,27 +1879,27 @@
   <dimension ref="A1:BM40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AQ3" sqref="AQ3"/>
+      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="34" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="2.7109375" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" hidden="1" customWidth="1"/>
-    <col min="10" max="65" width="2.5703125" customWidth="1"/>
-    <col min="67" max="67" width="9.140625" customWidth="1"/>
-    <col min="70" max="71" width="10.28515625"/>
+    <col min="1" max="1" width="2.6640625" style="34" customWidth="1"/>
+    <col min="2" max="2" width="38.44140625" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" customWidth="1"/>
+    <col min="8" max="8" width="2.6640625" customWidth="1"/>
+    <col min="9" max="9" width="6.109375" hidden="1" customWidth="1"/>
+    <col min="10" max="65" width="2.5546875" customWidth="1"/>
+    <col min="67" max="67" width="9.109375" customWidth="1"/>
+    <col min="70" max="71" width="10.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
@@ -1914,7 +1914,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="11"/>
     </row>
-    <row r="2" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="34" t="s">
         <v>1</v>
       </c>
@@ -1923,7 +1923,7 @@
       </c>
       <c r="J2" s="37"/>
     </row>
-    <row r="3" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
@@ -1936,12 +1936,12 @@
       <c r="D3" s="74"/>
       <c r="E3" s="75"/>
       <c r="F3" s="73">
-        <f ca="1">TODAY()+14</f>
-        <v>44379</v>
+        <f ca="1">TODAY()-4</f>
+        <v>44366</v>
       </c>
       <c r="G3" s="73"/>
     </row>
-    <row r="4" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
@@ -1958,7 +1958,7 @@
       </c>
       <c r="J4" s="70">
         <f ca="1">J5</f>
-        <v>44375</v>
+        <v>44361</v>
       </c>
       <c r="K4" s="71"/>
       <c r="L4" s="71"/>
@@ -1968,7 +1968,7 @@
       <c r="P4" s="72"/>
       <c r="Q4" s="70">
         <f ca="1">Q5</f>
-        <v>44382</v>
+        <v>44368</v>
       </c>
       <c r="R4" s="71"/>
       <c r="S4" s="71"/>
@@ -1978,7 +1978,7 @@
       <c r="W4" s="72"/>
       <c r="X4" s="70">
         <f ca="1">X5</f>
-        <v>44389</v>
+        <v>44375</v>
       </c>
       <c r="Y4" s="71"/>
       <c r="Z4" s="71"/>
@@ -1988,7 +1988,7 @@
       <c r="AD4" s="72"/>
       <c r="AE4" s="70">
         <f ca="1">AE5</f>
-        <v>44396</v>
+        <v>44382</v>
       </c>
       <c r="AF4" s="71"/>
       <c r="AG4" s="71"/>
@@ -1998,7 +1998,7 @@
       <c r="AK4" s="72"/>
       <c r="AL4" s="70">
         <f ca="1">AL5</f>
-        <v>44403</v>
+        <v>44389</v>
       </c>
       <c r="AM4" s="71"/>
       <c r="AN4" s="71"/>
@@ -2008,7 +2008,7 @@
       <c r="AR4" s="72"/>
       <c r="AS4" s="70">
         <f ca="1">AS5</f>
-        <v>44410</v>
+        <v>44396</v>
       </c>
       <c r="AT4" s="71"/>
       <c r="AU4" s="71"/>
@@ -2018,7 +2018,7 @@
       <c r="AY4" s="72"/>
       <c r="AZ4" s="70">
         <f ca="1">AZ5</f>
-        <v>44417</v>
+        <v>44403</v>
       </c>
       <c r="BA4" s="71"/>
       <c r="BB4" s="71"/>
@@ -2028,7 +2028,7 @@
       <c r="BF4" s="72"/>
       <c r="BG4" s="70">
         <f ca="1">BG5</f>
-        <v>44424</v>
+        <v>44410</v>
       </c>
       <c r="BH4" s="71"/>
       <c r="BI4" s="71"/>
@@ -2037,7 +2037,7 @@
       <c r="BL4" s="71"/>
       <c r="BM4" s="72"/>
     </row>
-    <row r="5" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="35" t="s">
         <v>4</v>
       </c>
@@ -2050,230 +2050,230 @@
       <c r="H5" s="76"/>
       <c r="J5" s="56">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>44375</v>
+        <v>44361</v>
       </c>
       <c r="K5" s="57">
         <f ca="1">J5+1</f>
-        <v>44376</v>
+        <v>44362</v>
       </c>
       <c r="L5" s="57">
         <f t="shared" ref="L5:AY5" ca="1" si="0">K5+1</f>
-        <v>44377</v>
+        <v>44363</v>
       </c>
       <c r="M5" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44378</v>
+        <v>44364</v>
       </c>
       <c r="N5" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44379</v>
+        <v>44365</v>
       </c>
       <c r="O5" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44380</v>
+        <v>44366</v>
       </c>
       <c r="P5" s="58">
         <f t="shared" ca="1" si="0"/>
-        <v>44381</v>
+        <v>44367</v>
       </c>
       <c r="Q5" s="56">
         <f ca="1">P5+1</f>
-        <v>44382</v>
+        <v>44368</v>
       </c>
       <c r="R5" s="57">
         <f ca="1">Q5+1</f>
-        <v>44383</v>
+        <v>44369</v>
       </c>
       <c r="S5" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44384</v>
+        <v>44370</v>
       </c>
       <c r="T5" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44385</v>
+        <v>44371</v>
       </c>
       <c r="U5" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44386</v>
+        <v>44372</v>
       </c>
       <c r="V5" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44387</v>
+        <v>44373</v>
       </c>
       <c r="W5" s="58">
         <f t="shared" ca="1" si="0"/>
-        <v>44388</v>
+        <v>44374</v>
       </c>
       <c r="X5" s="56">
         <f ca="1">W5+1</f>
-        <v>44389</v>
+        <v>44375</v>
       </c>
       <c r="Y5" s="57">
         <f ca="1">X5+1</f>
-        <v>44390</v>
+        <v>44376</v>
       </c>
       <c r="Z5" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44391</v>
+        <v>44377</v>
       </c>
       <c r="AA5" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44392</v>
+        <v>44378</v>
       </c>
       <c r="AB5" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44393</v>
+        <v>44379</v>
       </c>
       <c r="AC5" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44394</v>
+        <v>44380</v>
       </c>
       <c r="AD5" s="58">
         <f t="shared" ca="1" si="0"/>
-        <v>44395</v>
+        <v>44381</v>
       </c>
       <c r="AE5" s="56">
         <f ca="1">AD5+1</f>
-        <v>44396</v>
+        <v>44382</v>
       </c>
       <c r="AF5" s="57">
         <f ca="1">AE5+1</f>
-        <v>44397</v>
+        <v>44383</v>
       </c>
       <c r="AG5" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44398</v>
+        <v>44384</v>
       </c>
       <c r="AH5" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44399</v>
+        <v>44385</v>
       </c>
       <c r="AI5" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44400</v>
+        <v>44386</v>
       </c>
       <c r="AJ5" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44401</v>
+        <v>44387</v>
       </c>
       <c r="AK5" s="58">
         <f t="shared" ca="1" si="0"/>
-        <v>44402</v>
+        <v>44388</v>
       </c>
       <c r="AL5" s="56">
         <f ca="1">AK5+1</f>
-        <v>44403</v>
+        <v>44389</v>
       </c>
       <c r="AM5" s="57">
         <f ca="1">AL5+1</f>
-        <v>44404</v>
+        <v>44390</v>
       </c>
       <c r="AN5" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44405</v>
+        <v>44391</v>
       </c>
       <c r="AO5" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44406</v>
+        <v>44392</v>
       </c>
       <c r="AP5" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44407</v>
+        <v>44393</v>
       </c>
       <c r="AQ5" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44408</v>
+        <v>44394</v>
       </c>
       <c r="AR5" s="58">
         <f t="shared" ca="1" si="0"/>
-        <v>44409</v>
+        <v>44395</v>
       </c>
       <c r="AS5" s="56">
         <f ca="1">AR5+1</f>
-        <v>44410</v>
+        <v>44396</v>
       </c>
       <c r="AT5" s="57">
         <f ca="1">AS5+1</f>
-        <v>44411</v>
+        <v>44397</v>
       </c>
       <c r="AU5" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44398</v>
       </c>
       <c r="AV5" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44413</v>
+        <v>44399</v>
       </c>
       <c r="AW5" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44414</v>
+        <v>44400</v>
       </c>
       <c r="AX5" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44415</v>
+        <v>44401</v>
       </c>
       <c r="AY5" s="58">
         <f t="shared" ca="1" si="0"/>
-        <v>44416</v>
+        <v>44402</v>
       </c>
       <c r="AZ5" s="56">
         <f ca="1">AY5+1</f>
-        <v>44417</v>
+        <v>44403</v>
       </c>
       <c r="BA5" s="57">
         <f ca="1">AZ5+1</f>
-        <v>44418</v>
+        <v>44404</v>
       </c>
       <c r="BB5" s="57">
         <f t="shared" ref="BB5:BF5" ca="1" si="1">BA5+1</f>
-        <v>44419</v>
+        <v>44405</v>
       </c>
       <c r="BC5" s="57">
         <f t="shared" ca="1" si="1"/>
-        <v>44420</v>
+        <v>44406</v>
       </c>
       <c r="BD5" s="57">
         <f t="shared" ca="1" si="1"/>
-        <v>44421</v>
+        <v>44407</v>
       </c>
       <c r="BE5" s="57">
         <f t="shared" ca="1" si="1"/>
-        <v>44422</v>
+        <v>44408</v>
       </c>
       <c r="BF5" s="58">
         <f t="shared" ca="1" si="1"/>
-        <v>44423</v>
+        <v>44409</v>
       </c>
       <c r="BG5" s="56">
         <f ca="1">BF5+1</f>
-        <v>44424</v>
+        <v>44410</v>
       </c>
       <c r="BH5" s="57">
         <f ca="1">BG5+1</f>
-        <v>44425</v>
+        <v>44411</v>
       </c>
       <c r="BI5" s="57">
         <f t="shared" ref="BI5:BM5" ca="1" si="2">BH5+1</f>
-        <v>44426</v>
+        <v>44412</v>
       </c>
       <c r="BJ5" s="57">
         <f t="shared" ca="1" si="2"/>
-        <v>44427</v>
+        <v>44413</v>
       </c>
       <c r="BK5" s="57">
         <f t="shared" ca="1" si="2"/>
-        <v>44428</v>
+        <v>44414</v>
       </c>
       <c r="BL5" s="57">
         <f t="shared" ca="1" si="2"/>
-        <v>44429</v>
+        <v>44415</v>
       </c>
       <c r="BM5" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>44430</v>
-      </c>
-    </row>
-    <row r="6" spans="1:65" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>44416</v>
+      </c>
+    </row>
+    <row r="6" spans="1:65" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="35" t="s">
         <v>5</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="7" spans="1:65" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:65" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="34" t="s">
         <v>6</v>
       </c>
@@ -2592,7 +2592,7 @@
       <c r="BL7" s="63"/>
       <c r="BM7" s="63"/>
     </row>
-    <row r="8" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="35" t="s">
         <v>7</v>
       </c>
@@ -2663,7 +2663,7 @@
       <c r="BL8"/>
       <c r="BM8"/>
     </row>
-    <row r="9" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="35" t="s">
         <v>8</v>
       </c>
@@ -2681,11 +2681,11 @@
       </c>
       <c r="F9" s="59">
         <f ca="1">Project_Start</f>
-        <v>44379</v>
+        <v>44366</v>
       </c>
       <c r="G9" s="59">
         <f ca="1">F9+2</f>
-        <v>44381</v>
+        <v>44368</v>
       </c>
       <c r="H9" s="64"/>
       <c r="I9" s="64"/>
@@ -2746,7 +2746,7 @@
       <c r="BL9" s="64"/>
       <c r="BM9" s="64"/>
     </row>
-    <row r="10" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="35" t="s">
         <v>9</v>
       </c>
@@ -2764,11 +2764,11 @@
       </c>
       <c r="F10" s="59">
         <f ca="1">Project_Start</f>
-        <v>44379</v>
+        <v>44366</v>
       </c>
       <c r="G10" s="59">
         <f ca="1">F10+4</f>
-        <v>44383</v>
+        <v>44370</v>
       </c>
       <c r="H10" s="64"/>
       <c r="I10" s="64"/>
@@ -2829,7 +2829,7 @@
       <c r="BL10" s="64"/>
       <c r="BM10" s="64"/>
     </row>
-    <row r="11" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="34"/>
       <c r="B11" s="46" t="s">
         <v>45</v>
@@ -2841,15 +2841,15 @@
         <v>5</v>
       </c>
       <c r="E11" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="59">
         <f ca="1">Project_Start</f>
-        <v>44379</v>
+        <v>44366</v>
       </c>
       <c r="G11" s="59">
         <f ca="1">F11+2</f>
-        <v>44381</v>
+        <v>44368</v>
       </c>
       <c r="H11" s="64"/>
       <c r="I11" s="64"/>
@@ -2910,7 +2910,7 @@
       <c r="BL11" s="64"/>
       <c r="BM11" s="64"/>
     </row>
-    <row r="12" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="34"/>
       <c r="B12" s="46" t="s">
         <v>48</v>
@@ -2922,15 +2922,15 @@
         <v>5</v>
       </c>
       <c r="E12" s="16">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F12" s="59">
         <f ca="1">G11+3</f>
-        <v>44384</v>
+        <v>44371</v>
       </c>
       <c r="G12" s="59">
         <f ca="1">F12+1</f>
-        <v>44385</v>
+        <v>44372</v>
       </c>
       <c r="H12" s="64"/>
       <c r="I12" s="64"/>
@@ -2991,7 +2991,7 @@
       <c r="BL12" s="64"/>
       <c r="BM12" s="64"/>
     </row>
-    <row r="13" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="34"/>
       <c r="B13" s="46" t="s">
         <v>53</v>
@@ -3007,11 +3007,11 @@
       </c>
       <c r="F13" s="59">
         <f ca="1">G12+1</f>
-        <v>44386</v>
+        <v>44373</v>
       </c>
       <c r="G13" s="59">
         <f ca="1">F13+2</f>
-        <v>44388</v>
+        <v>44375</v>
       </c>
       <c r="H13" s="64"/>
       <c r="I13" s="64"/>
@@ -3072,7 +3072,7 @@
       <c r="BL13" s="64"/>
       <c r="BM13" s="64"/>
     </row>
-    <row r="14" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="35" t="s">
         <v>10</v>
       </c>
@@ -3090,11 +3090,11 @@
       </c>
       <c r="F14" s="59">
         <f ca="1">G10+1</f>
-        <v>44384</v>
+        <v>44371</v>
       </c>
       <c r="G14" s="59">
         <f ca="1">F14+6</f>
-        <v>44390</v>
+        <v>44377</v>
       </c>
       <c r="H14" s="64"/>
       <c r="I14" s="64"/>
@@ -3155,7 +3155,7 @@
       <c r="BL14" s="64"/>
       <c r="BM14" s="64"/>
     </row>
-    <row r="15" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="35"/>
       <c r="B15" s="46" t="s">
         <v>46</v>
@@ -3171,11 +3171,11 @@
       </c>
       <c r="F15" s="59">
         <f ca="1">G14+1</f>
-        <v>44391</v>
+        <v>44378</v>
       </c>
       <c r="G15" s="59">
         <f ca="1">F15+1</f>
-        <v>44392</v>
+        <v>44379</v>
       </c>
       <c r="H15" s="64"/>
       <c r="I15" s="64"/>
@@ -3236,7 +3236,7 @@
       <c r="BL15" s="64"/>
       <c r="BM15" s="64"/>
     </row>
-    <row r="16" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="34"/>
       <c r="B16" s="46" t="s">
         <v>47</v>
@@ -3252,11 +3252,11 @@
       </c>
       <c r="F16" s="59">
         <f ca="1">G15+1</f>
-        <v>44393</v>
+        <v>44380</v>
       </c>
       <c r="G16" s="59">
         <f ca="1">F16+1</f>
-        <v>44394</v>
+        <v>44381</v>
       </c>
       <c r="H16" s="64"/>
       <c r="I16" s="64"/>
@@ -3317,7 +3317,7 @@
       <c r="BL16" s="64"/>
       <c r="BM16" s="64"/>
     </row>
-    <row r="17" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="34"/>
       <c r="B17" s="46" t="s">
         <v>54</v>
@@ -3333,11 +3333,11 @@
       </c>
       <c r="F17" s="59">
         <f ca="1">G16+1</f>
-        <v>44395</v>
+        <v>44382</v>
       </c>
       <c r="G17" s="59">
         <f ca="1">F17+2</f>
-        <v>44397</v>
+        <v>44384</v>
       </c>
       <c r="H17" s="64"/>
       <c r="I17" s="64"/>
@@ -3398,7 +3398,7 @@
       <c r="BL17" s="64"/>
       <c r="BM17" s="64"/>
     </row>
-    <row r="18" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="34"/>
       <c r="B18" s="17" t="s">
         <v>61</v>
@@ -3467,7 +3467,7 @@
       <c r="BL18"/>
       <c r="BM18"/>
     </row>
-    <row r="19" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="34"/>
       <c r="B19" s="47" t="s">
         <v>52</v>
@@ -3483,11 +3483,11 @@
       </c>
       <c r="F19" s="60">
         <f ca="1">G17+1</f>
-        <v>44398</v>
+        <v>44385</v>
       </c>
       <c r="G19" s="60">
         <f ca="1">F19+2</f>
-        <v>44400</v>
+        <v>44387</v>
       </c>
       <c r="H19" s="64"/>
       <c r="I19" s="64"/>
@@ -3548,7 +3548,7 @@
       <c r="BL19" s="64"/>
       <c r="BM19" s="64"/>
     </row>
-    <row r="20" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="34" t="s">
         <v>11</v>
       </c>
@@ -3566,11 +3566,11 @@
       </c>
       <c r="F20" s="60">
         <f ca="1">G16+1</f>
-        <v>44395</v>
+        <v>44382</v>
       </c>
       <c r="G20" s="60">
         <f ca="1">F20+3</f>
-        <v>44398</v>
+        <v>44385</v>
       </c>
       <c r="H20" s="64"/>
       <c r="I20" s="64"/>
@@ -3631,7 +3631,7 @@
       <c r="BL20" s="64"/>
       <c r="BM20" s="64"/>
     </row>
-    <row r="21" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="34"/>
       <c r="B21" s="47" t="s">
         <v>55</v>
@@ -3647,11 +3647,11 @@
       </c>
       <c r="F21" s="60">
         <f ca="1">G14+1</f>
-        <v>44391</v>
+        <v>44378</v>
       </c>
       <c r="G21" s="60">
         <f ca="1">F21+11</f>
-        <v>44402</v>
+        <v>44389</v>
       </c>
       <c r="H21" s="64"/>
       <c r="I21" s="64"/>
@@ -3712,7 +3712,7 @@
       <c r="BL21" s="64"/>
       <c r="BM21" s="64"/>
     </row>
-    <row r="22" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="34"/>
       <c r="B22" s="47" t="s">
         <v>56</v>
@@ -3728,11 +3728,11 @@
       </c>
       <c r="F22" s="60">
         <f ca="1">G17+1</f>
-        <v>44398</v>
+        <v>44385</v>
       </c>
       <c r="G22" s="60">
         <f ca="1">F22+11</f>
-        <v>44409</v>
+        <v>44396</v>
       </c>
       <c r="H22" s="64"/>
       <c r="I22" s="64"/>
@@ -3793,7 +3793,7 @@
       <c r="BL22" s="64"/>
       <c r="BM22" s="64"/>
     </row>
-    <row r="23" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="34"/>
       <c r="B23" s="47" t="s">
         <v>58</v>
@@ -3809,11 +3809,11 @@
       </c>
       <c r="F23" s="60">
         <f ca="1">G22</f>
-        <v>44409</v>
+        <v>44396</v>
       </c>
       <c r="G23" s="60">
         <f ca="1">F23+1</f>
-        <v>44410</v>
+        <v>44397</v>
       </c>
       <c r="H23" s="64"/>
       <c r="I23" s="64"/>
@@ -3874,7 +3874,7 @@
       <c r="BL23" s="64"/>
       <c r="BM23" s="64"/>
     </row>
-    <row r="24" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="34"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -3941,7 +3941,7 @@
       <c r="BL24"/>
       <c r="BM24"/>
     </row>
-    <row r="25" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="34"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -4008,7 +4008,7 @@
       <c r="BL25"/>
       <c r="BM25"/>
     </row>
-    <row r="26" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="34" t="s">
         <v>11</v>
       </c>
@@ -4077,7 +4077,7 @@
       <c r="BL26"/>
       <c r="BM26"/>
     </row>
-    <row r="27" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="34"/>
       <c r="B27"/>
       <c r="C27"/>
@@ -4144,7 +4144,7 @@
       <c r="BL27"/>
       <c r="BM27"/>
     </row>
-    <row r="28" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="34"/>
       <c r="B28"/>
       <c r="C28"/>
@@ -4211,7 +4211,7 @@
       <c r="BL28"/>
       <c r="BM28"/>
     </row>
-    <row r="29" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="34"/>
       <c r="B29"/>
       <c r="C29"/>
@@ -4278,7 +4278,7 @@
       <c r="BL29"/>
       <c r="BM29"/>
     </row>
-    <row r="30" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="34"/>
       <c r="B30"/>
       <c r="C30"/>
@@ -4345,7 +4345,7 @@
       <c r="BL30"/>
       <c r="BM30"/>
     </row>
-    <row r="31" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="34"/>
       <c r="B31"/>
       <c r="C31"/>
@@ -4412,7 +4412,7 @@
       <c r="BL31"/>
       <c r="BM31"/>
     </row>
-    <row r="32" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="34" t="s">
         <v>12</v>
       </c>
@@ -4481,7 +4481,7 @@
       <c r="BL32"/>
       <c r="BM32"/>
     </row>
-    <row r="33" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="35" t="s">
         <v>13</v>
       </c>
@@ -4550,14 +4550,14 @@
       <c r="BL33"/>
       <c r="BM33"/>
     </row>
-    <row r="34" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F34"/>
       <c r="H34" s="6"/>
     </row>
-    <row r="35" spans="1:65" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:65" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F35"/>
     </row>
-    <row r="36" spans="1:65" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:65" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="48"/>
       <c r="C36" s="45"/>
       <c r="D36" s="45"/>
@@ -4565,7 +4565,7 @@
       <c r="F36" s="53"/>
       <c r="G36" s="53"/>
     </row>
-    <row r="37" spans="1:65" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:65" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="20" t="s">
         <v>15</v>
       </c>
@@ -4575,12 +4575,12 @@
       <c r="F37" s="54"/>
       <c r="G37" s="55"/>
     </row>
-    <row r="39" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
       <c r="G39" s="36"/>
     </row>
-    <row r="40" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
     </row>
@@ -4673,86 +4673,86 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="98.42578125" style="24" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="98.44140625" style="24" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:2" s="26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:2" s="26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="25"/>
     </row>
-    <row r="3" spans="1:2" s="30" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="30" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="31"/>
     </row>
-    <row r="4" spans="1:2" s="27" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" s="27" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A4" s="28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="24" customFormat="1" ht="204.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" s="24" customFormat="1" ht="204.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="27" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:2" s="27" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A8" s="28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="24" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" s="24" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="27" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:2" s="27" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A11" s="28" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="24" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" s="24" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="27" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:2" s="27" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A14" s="28" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="90" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
         <v>36</v>
       </c>

</xml_diff>